<commit_message>
ticket 171: quitado ID_SERVICIO de plantillas y puesto ID_ORDEN_SERVICIO
</commit_message>
<xml_diff>
--- a/public/uploads/${ID_ORDEN_SERVICIO} ORDEN DE SERVICIO NEDETEL S A aumento ${NODO_CIU_NOMBRE} ${INICIALES_CLIENTE}.xlsx
+++ b/public/uploads/${ID_ORDEN_SERVICIO} ORDEN DE SERVICIO NEDETEL S A aumento ${NODO_CIU_NOMBRE} ${INICIALES_CLIENTE}.xlsx
@@ -22,7 +22,35 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="130">
   <si>
-    <t xml:space="preserve">ORDEN DE SERVICIO ${ID_SERVICIO}</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="24"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ORDEN DE SERVICIO ${ID_</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="24"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ORDEN_</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="24"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SERVICIO}</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">FOR GCO UIO 01 ORDEN DE SERVICIO ver 11 01 08</t>
@@ -425,7 +453,7 @@
     <numFmt numFmtId="169" formatCode="0.00\ %"/>
     <numFmt numFmtId="170" formatCode="&quot;$ &quot;#,##0.00"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -453,6 +481,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -760,15 +794,15 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="110">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -785,379 +819,343 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="12" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1165,27 +1163,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1193,31 +1191,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1225,15 +1207,31 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1241,7 +1239,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1270,9 +1268,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>2015640</xdr:colOff>
+      <xdr:colOff>2015280</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1286,7 +1284,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16530840" y="16480080"/>
-          <a:ext cx="1873800" cy="968760"/>
+          <a:ext cx="1873440" cy="968400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1309,7 +1307,7 @@
   <dimension ref="A1:V71"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -2452,203 +2450,203 @@
       <c r="F44" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="G44" s="67" t="s">
+      <c r="G44" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="H44" s="67" t="s">
+      <c r="H44" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="I44" s="67" t="s">
+      <c r="I44" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="J44" s="67" t="s">
+      <c r="J44" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="K44" s="68" t="n">
+      <c r="K44" s="67" t="n">
         <v>0.995</v>
       </c>
-      <c r="L44" s="67" t="s">
+      <c r="L44" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="M44" s="67" t="s">
+      <c r="M44" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="N44" s="67" t="s">
+      <c r="N44" s="62" t="s">
         <v>99</v>
       </c>
-      <c r="O44" s="67" t="s">
+      <c r="O44" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="P44" s="67" t="s">
+      <c r="P44" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="Q44" s="67" t="s">
+      <c r="Q44" s="62" t="s">
         <v>57</v>
       </c>
       <c r="R44" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="S44" s="69" t="s">
+      <c r="S44" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="T44" s="70" t="s">
+      <c r="T44" s="69" t="s">
         <v>103</v>
       </c>
-      <c r="U44" s="71"/>
-      <c r="V44" s="72" t="s">
+      <c r="U44" s="8"/>
+      <c r="V44" s="70" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="45" s="1" customFormat="true" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="58"/>
       <c r="B45" s="62"/>
-      <c r="C45" s="73"/>
-      <c r="D45" s="74"/>
-      <c r="E45" s="75"/>
-      <c r="F45" s="76"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="72"/>
+      <c r="E45" s="65"/>
+      <c r="F45" s="66"/>
       <c r="G45" s="62"/>
       <c r="H45" s="62"/>
       <c r="I45" s="62"/>
       <c r="J45" s="62"/>
-      <c r="K45" s="77"/>
+      <c r="K45" s="67"/>
       <c r="L45" s="62"/>
       <c r="M45" s="62"/>
       <c r="N45" s="62"/>
       <c r="O45" s="62"/>
       <c r="P45" s="62"/>
       <c r="Q45" s="62"/>
-      <c r="R45" s="78"/>
-      <c r="S45" s="79"/>
-      <c r="T45" s="80"/>
+      <c r="R45" s="64"/>
+      <c r="S45" s="68"/>
+      <c r="T45" s="69"/>
       <c r="U45" s="8"/>
       <c r="V45" s="8"/>
     </row>
     <row r="46" s="1" customFormat="true" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="58"/>
       <c r="B46" s="62"/>
-      <c r="C46" s="73"/>
-      <c r="D46" s="74"/>
-      <c r="E46" s="75"/>
-      <c r="F46" s="76"/>
+      <c r="C46" s="71"/>
+      <c r="D46" s="72"/>
+      <c r="E46" s="65"/>
+      <c r="F46" s="66"/>
       <c r="G46" s="62"/>
       <c r="H46" s="62"/>
       <c r="I46" s="62"/>
       <c r="J46" s="62"/>
-      <c r="K46" s="77"/>
+      <c r="K46" s="67"/>
       <c r="L46" s="62"/>
       <c r="M46" s="62"/>
       <c r="N46" s="62"/>
       <c r="O46" s="62"/>
       <c r="P46" s="62"/>
       <c r="Q46" s="62"/>
-      <c r="R46" s="78"/>
-      <c r="S46" s="79"/>
-      <c r="T46" s="80"/>
+      <c r="R46" s="64"/>
+      <c r="S46" s="68"/>
+      <c r="T46" s="69"/>
       <c r="U46" s="8"/>
-      <c r="V46" s="81"/>
+      <c r="V46" s="70"/>
     </row>
     <row r="47" s="1" customFormat="true" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="58"/>
       <c r="B47" s="62"/>
       <c r="C47" s="62"/>
-      <c r="D47" s="74"/>
+      <c r="D47" s="72"/>
       <c r="E47" s="25"/>
       <c r="F47" s="62"/>
       <c r="G47" s="62"/>
       <c r="H47" s="62"/>
       <c r="I47" s="62"/>
       <c r="J47" s="62"/>
-      <c r="K47" s="77"/>
+      <c r="K47" s="67"/>
       <c r="L47" s="62"/>
       <c r="M47" s="62"/>
       <c r="N47" s="62"/>
       <c r="O47" s="62"/>
       <c r="P47" s="62"/>
       <c r="Q47" s="62"/>
-      <c r="R47" s="78"/>
-      <c r="S47" s="82"/>
-      <c r="T47" s="82"/>
+      <c r="R47" s="64"/>
+      <c r="S47" s="73"/>
+      <c r="T47" s="73"/>
       <c r="U47" s="8"/>
-      <c r="V47" s="81"/>
+      <c r="V47" s="70"/>
     </row>
     <row r="48" s="1" customFormat="true" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="58"/>
       <c r="B48" s="62"/>
       <c r="C48" s="62"/>
-      <c r="D48" s="74"/>
+      <c r="D48" s="72"/>
       <c r="E48" s="25"/>
       <c r="F48" s="62"/>
       <c r="G48" s="62"/>
       <c r="H48" s="62"/>
       <c r="I48" s="62"/>
       <c r="J48" s="62"/>
-      <c r="K48" s="77"/>
+      <c r="K48" s="67"/>
       <c r="L48" s="62"/>
       <c r="M48" s="62"/>
       <c r="N48" s="62"/>
       <c r="O48" s="62"/>
       <c r="P48" s="62"/>
       <c r="Q48" s="62"/>
-      <c r="R48" s="78"/>
-      <c r="S48" s="82"/>
-      <c r="T48" s="82"/>
+      <c r="R48" s="64"/>
+      <c r="S48" s="73"/>
+      <c r="T48" s="73"/>
       <c r="U48" s="8"/>
-      <c r="V48" s="81"/>
+      <c r="V48" s="70"/>
     </row>
     <row r="49" customFormat="false" ht="57.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R49" s="83" t="s">
+      <c r="R49" s="74" t="s">
         <v>105</v>
       </c>
-      <c r="S49" s="80" t="s">
+      <c r="S49" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="T49" s="80" t="s">
+      <c r="T49" s="69" t="s">
         <v>103</v>
       </c>
-      <c r="U49" s="84"/>
+      <c r="U49" s="75"/>
     </row>
     <row r="50" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R50" s="83" t="s">
+      <c r="R50" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="S50" s="80" t="s">
+      <c r="S50" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="T50" s="80" t="s">
+      <c r="T50" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="U50" s="84"/>
+      <c r="U50" s="75"/>
     </row>
     <row r="51" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R51" s="83" t="s">
+      <c r="R51" s="74" t="s">
         <v>109</v>
       </c>
-      <c r="S51" s="80" t="s">
+      <c r="S51" s="69" t="s">
         <v>110</v>
       </c>
-      <c r="T51" s="80" t="s">
+      <c r="T51" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="U51" s="84"/>
+      <c r="U51" s="75"/>
     </row>
     <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="85"/>
-      <c r="C52" s="85"/>
-      <c r="D52" s="85"/>
+      <c r="B52" s="76"/>
+      <c r="C52" s="76"/>
+      <c r="D52" s="76"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
-      <c r="G52" s="86"/>
-      <c r="H52" s="86"/>
-      <c r="I52" s="86"/>
-      <c r="J52" s="86"/>
-      <c r="K52" s="86"/>
-      <c r="L52" s="86"/>
-      <c r="M52" s="86"/>
-      <c r="N52" s="86"/>
-      <c r="O52" s="86"/>
-      <c r="P52" s="86"/>
-      <c r="Q52" s="86"/>
-      <c r="R52" s="85"/>
+      <c r="G52" s="77"/>
+      <c r="H52" s="77"/>
+      <c r="I52" s="77"/>
+      <c r="J52" s="77"/>
+      <c r="K52" s="77"/>
+      <c r="L52" s="77"/>
+      <c r="M52" s="77"/>
+      <c r="N52" s="77"/>
+      <c r="O52" s="77"/>
+      <c r="P52" s="77"/>
+      <c r="Q52" s="77"/>
+      <c r="R52" s="76"/>
     </row>
     <row r="53" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="57"/>
@@ -2671,11 +2669,11 @@
       <c r="P53" s="11"/>
       <c r="Q53" s="11"/>
       <c r="R53" s="11"/>
-      <c r="S53" s="87"/>
-      <c r="T53" s="87"/>
+      <c r="S53" s="78"/>
+      <c r="T53" s="78"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="88"/>
+      <c r="B54" s="79"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B55" s="61" t="s">
@@ -2687,195 +2685,195 @@
       </c>
       <c r="E55" s="61"/>
       <c r="F55" s="61"/>
-      <c r="G55" s="89" t="s">
+      <c r="G55" s="80" t="s">
         <v>115</v>
       </c>
-      <c r="H55" s="90"/>
-      <c r="I55" s="91" t="s">
+      <c r="H55" s="81"/>
+      <c r="I55" s="82" t="s">
         <v>116</v>
       </c>
-      <c r="J55" s="91"/>
-      <c r="K55" s="90"/>
-      <c r="L55" s="90"/>
-      <c r="M55" s="92" t="s">
+      <c r="J55" s="82"/>
+      <c r="K55" s="81"/>
+      <c r="L55" s="81"/>
+      <c r="M55" s="83" t="s">
         <v>117</v>
       </c>
-      <c r="N55" s="92"/>
-      <c r="O55" s="92"/>
-      <c r="P55" s="92"/>
-      <c r="Q55" s="92"/>
-      <c r="R55" s="92"/>
+      <c r="N55" s="83"/>
+      <c r="O55" s="83"/>
+      <c r="P55" s="83"/>
+      <c r="Q55" s="83"/>
+      <c r="R55" s="83"/>
     </row>
     <row r="56" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B56" s="93"/>
-      <c r="C56" s="93"/>
-      <c r="D56" s="94"/>
-      <c r="E56" s="94"/>
-      <c r="F56" s="94"/>
-      <c r="G56" s="75"/>
-      <c r="H56" s="95"/>
-      <c r="I56" s="95"/>
-      <c r="J56" s="95"/>
-      <c r="K56" s="96"/>
-      <c r="L56" s="96"/>
-      <c r="M56" s="97"/>
-      <c r="N56" s="97"/>
-      <c r="O56" s="97"/>
-      <c r="P56" s="97"/>
-      <c r="Q56" s="97"/>
-      <c r="R56" s="98"/>
+      <c r="B56" s="84"/>
+      <c r="C56" s="84"/>
+      <c r="D56" s="85"/>
+      <c r="E56" s="85"/>
+      <c r="F56" s="85"/>
+      <c r="G56" s="65"/>
+      <c r="H56" s="86"/>
+      <c r="I56" s="86"/>
+      <c r="J56" s="86"/>
+      <c r="K56" s="87"/>
+      <c r="L56" s="87"/>
+      <c r="M56" s="88"/>
+      <c r="N56" s="88"/>
+      <c r="O56" s="88"/>
+      <c r="P56" s="88"/>
+      <c r="Q56" s="88"/>
+      <c r="R56" s="89"/>
     </row>
     <row r="57" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B57" s="99" t="s">
+      <c r="B57" s="90" t="s">
         <v>120</v>
       </c>
-      <c r="C57" s="99"/>
-      <c r="D57" s="100" t="s">
+      <c r="C57" s="90"/>
+      <c r="D57" s="91" t="s">
         <v>121</v>
       </c>
-      <c r="E57" s="100"/>
-      <c r="F57" s="100"/>
-      <c r="G57" s="101" t="s">
+      <c r="E57" s="91"/>
+      <c r="F57" s="91"/>
+      <c r="G57" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="H57" s="102" t="s">
+      <c r="H57" s="93" t="s">
         <v>122</v>
       </c>
-      <c r="I57" s="102"/>
-      <c r="J57" s="102"/>
-      <c r="K57" s="103"/>
-      <c r="L57" s="103"/>
-      <c r="M57" s="104"/>
-      <c r="N57" s="104"/>
-      <c r="O57" s="104"/>
-      <c r="P57" s="104"/>
-      <c r="Q57" s="104"/>
-      <c r="R57" s="105"/>
+      <c r="I57" s="93"/>
+      <c r="J57" s="93"/>
+      <c r="K57" s="94"/>
+      <c r="L57" s="94"/>
+      <c r="M57" s="95"/>
+      <c r="N57" s="95"/>
+      <c r="O57" s="95"/>
+      <c r="P57" s="95"/>
+      <c r="Q57" s="95"/>
+      <c r="R57" s="96"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B58" s="99"/>
-      <c r="C58" s="99"/>
-      <c r="D58" s="100"/>
-      <c r="E58" s="100"/>
-      <c r="F58" s="100"/>
-      <c r="G58" s="101"/>
-      <c r="H58" s="102"/>
-      <c r="I58" s="102"/>
-      <c r="J58" s="102"/>
-      <c r="K58" s="103"/>
-      <c r="L58" s="103"/>
-      <c r="M58" s="106"/>
-      <c r="N58" s="106"/>
-      <c r="O58" s="106"/>
-      <c r="P58" s="106"/>
-      <c r="Q58" s="106"/>
-      <c r="R58" s="105"/>
+      <c r="B58" s="90"/>
+      <c r="C58" s="90"/>
+      <c r="D58" s="91"/>
+      <c r="E58" s="91"/>
+      <c r="F58" s="91"/>
+      <c r="G58" s="92"/>
+      <c r="H58" s="93"/>
+      <c r="I58" s="93"/>
+      <c r="J58" s="93"/>
+      <c r="K58" s="94"/>
+      <c r="L58" s="94"/>
+      <c r="M58" s="97"/>
+      <c r="N58" s="97"/>
+      <c r="O58" s="97"/>
+      <c r="P58" s="97"/>
+      <c r="Q58" s="97"/>
+      <c r="R58" s="96"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="107"/>
-      <c r="C59" s="107"/>
-      <c r="D59" s="107"/>
-      <c r="E59" s="107"/>
-      <c r="F59" s="107"/>
-      <c r="G59" s="108"/>
-      <c r="H59" s="109"/>
-      <c r="I59" s="110"/>
-      <c r="J59" s="111"/>
-      <c r="K59" s="103"/>
-      <c r="L59" s="103"/>
-      <c r="M59" s="106"/>
-      <c r="N59" s="106"/>
-      <c r="O59" s="106"/>
-      <c r="P59" s="106"/>
-      <c r="Q59" s="106"/>
-      <c r="R59" s="105"/>
+      <c r="B59" s="98"/>
+      <c r="C59" s="98"/>
+      <c r="D59" s="98"/>
+      <c r="E59" s="98"/>
+      <c r="F59" s="98"/>
+      <c r="G59" s="99"/>
+      <c r="H59" s="100"/>
+      <c r="I59" s="101"/>
+      <c r="J59" s="102"/>
+      <c r="K59" s="94"/>
+      <c r="L59" s="94"/>
+      <c r="M59" s="97"/>
+      <c r="N59" s="97"/>
+      <c r="O59" s="97"/>
+      <c r="P59" s="97"/>
+      <c r="Q59" s="97"/>
+      <c r="R59" s="96"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B60" s="112"/>
-      <c r="C60" s="112"/>
-      <c r="D60" s="112"/>
-      <c r="E60" s="112"/>
-      <c r="F60" s="112"/>
-      <c r="G60" s="103"/>
-      <c r="H60" s="113"/>
-      <c r="I60" s="114"/>
-      <c r="J60" s="105"/>
-      <c r="K60" s="103"/>
-      <c r="L60" s="103"/>
-      <c r="M60" s="115"/>
-      <c r="N60" s="115"/>
-      <c r="O60" s="115"/>
-      <c r="P60" s="115"/>
-      <c r="Q60" s="115"/>
-      <c r="R60" s="105"/>
+      <c r="B60" s="103"/>
+      <c r="C60" s="103"/>
+      <c r="D60" s="103"/>
+      <c r="E60" s="103"/>
+      <c r="F60" s="103"/>
+      <c r="G60" s="94"/>
+      <c r="H60" s="104"/>
+      <c r="I60" s="105"/>
+      <c r="J60" s="96"/>
+      <c r="K60" s="94"/>
+      <c r="L60" s="94"/>
+      <c r="M60" s="106"/>
+      <c r="N60" s="106"/>
+      <c r="O60" s="106"/>
+      <c r="P60" s="106"/>
+      <c r="Q60" s="106"/>
+      <c r="R60" s="96"/>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B61" s="112"/>
-      <c r="C61" s="112"/>
-      <c r="D61" s="112"/>
-      <c r="E61" s="112"/>
-      <c r="F61" s="112"/>
-      <c r="G61" s="103"/>
-      <c r="H61" s="113"/>
-      <c r="I61" s="114"/>
-      <c r="J61" s="105"/>
-      <c r="K61" s="103"/>
-      <c r="L61" s="103"/>
-      <c r="M61" s="115"/>
-      <c r="N61" s="115"/>
-      <c r="O61" s="115"/>
-      <c r="P61" s="115"/>
-      <c r="Q61" s="115"/>
-      <c r="R61" s="105"/>
+      <c r="B61" s="103"/>
+      <c r="C61" s="103"/>
+      <c r="D61" s="103"/>
+      <c r="E61" s="103"/>
+      <c r="F61" s="103"/>
+      <c r="G61" s="94"/>
+      <c r="H61" s="104"/>
+      <c r="I61" s="105"/>
+      <c r="J61" s="96"/>
+      <c r="K61" s="94"/>
+      <c r="L61" s="94"/>
+      <c r="M61" s="106"/>
+      <c r="N61" s="106"/>
+      <c r="O61" s="106"/>
+      <c r="P61" s="106"/>
+      <c r="Q61" s="106"/>
+      <c r="R61" s="96"/>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="116"/>
-      <c r="C68" s="116"/>
-      <c r="D68" s="116"/>
-      <c r="E68" s="116"/>
-      <c r="F68" s="116"/>
+      <c r="B68" s="107"/>
+      <c r="C68" s="107"/>
+      <c r="D68" s="107"/>
+      <c r="E68" s="107"/>
+      <c r="F68" s="107"/>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C69" s="117"/>
-      <c r="R69" s="117"/>
+      <c r="C69" s="108"/>
+      <c r="R69" s="108"/>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C70" s="118" t="s">
+      <c r="C70" s="109" t="s">
         <v>127</v>
       </c>
-      <c r="D70" s="118"/>
-      <c r="E70" s="118"/>
-      <c r="F70" s="118"/>
-      <c r="R70" s="118" t="s">
+      <c r="D70" s="109"/>
+      <c r="E70" s="109"/>
+      <c r="F70" s="109"/>
+      <c r="R70" s="109" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C71" s="118" t="s">
+      <c r="C71" s="109" t="s">
         <v>129</v>
       </c>
-      <c r="D71" s="118"/>
-      <c r="E71" s="118"/>
-      <c r="F71" s="118"/>
-      <c r="R71" s="118" t="s">
+      <c r="D71" s="109"/>
+      <c r="E71" s="109"/>
+      <c r="F71" s="109"/>
+      <c r="R71" s="109" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>